<commit_message>
Add parameter settings for Minyue.
</commit_message>
<xml_diff>
--- a/中心线相机算法相关参数设置.xlsx
+++ b/中心线相机算法相关参数设置.xlsx
@@ -102,10 +102,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>ROI_EN</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>0x33bb0034</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -192,11 +188,15 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>0x33bb0200</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x33bb0204</t>
+    <t>ROI_EN</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x33bb0110</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x33bb0114</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -290,6 +290,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -298,9 +301,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -605,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -617,10 +617,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="4"/>
+      <c r="A1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="5"/>
     </row>
     <row r="2" spans="1:2" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
@@ -699,74 +699,74 @@
         <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="4"/>
+      <c r="B18" s="5"/>
     </row>
     <row r="19" spans="1:2" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="7" t="s">
         <v>38</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>0</v>
@@ -777,7 +777,7 @@
         <v>41</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="17.25" x14ac:dyDescent="0.15">
@@ -785,7 +785,7 @@
         <v>42</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
@@ -827,357 +827,357 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A1" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
+      <c r="A1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
     </row>
     <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
     </row>
     <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
     </row>
     <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
     </row>
     <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
     </row>
     <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
     </row>
     <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
     </row>
     <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
     </row>
     <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
     </row>
     <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
     </row>
     <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
     </row>
     <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
     </row>
     <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
     </row>
     <row r="37" spans="5:7" x14ac:dyDescent="0.15">
       <c r="E37">

</xml_diff>